<commit_message>
se añaden resultados experimento 2
</commit_message>
<xml_diff>
--- a/Parametros_entrenamientos.xlsx
+++ b/Parametros_entrenamientos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\julio\Documents\VIU\2425\TFM\codigo\trabajo aprendizaje refuerzo\git\Proyecto_programacion_APR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F3EB09C-9A7C-45BC-B63E-A0D64485DCCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7B0D4A-6002-49C3-ADDE-623A9FB51A45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="78">
   <si>
     <t>PRUEBAS</t>
   </si>
@@ -247,6 +247,18 @@
     <t xml:space="preserve">va subiendo un poco "linealmente"
 ligera mayor estabilidad que para los otros casos
 </t>
+  </si>
+  <si>
+    <t>num_episodes</t>
+  </si>
+  <si>
+    <t>112m 37 seg</t>
+  </si>
+  <si>
+    <t>7 ~ 23 | Media: 11.80</t>
+  </si>
+  <si>
+    <t>va subiendo mucho</t>
   </si>
 </sst>
 </file>
@@ -1139,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1151,7 +1163,8 @@
     <col min="2" max="2" width="22.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="14.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="14.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1396,6 +1409,9 @@
       <c r="D12" t="s">
         <v>71</v>
       </c>
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B13" t="s">
@@ -1407,6 +1423,9 @@
       <c r="D13" t="s">
         <v>70</v>
       </c>
+      <c r="E13" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B14" t="s">
@@ -1418,6 +1437,9 @@
       <c r="D14" t="s">
         <v>66</v>
       </c>
+      <c r="E14" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="15" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B15" s="4" t="s">
@@ -1429,6 +1451,9 @@
       <c r="D15" s="4" t="s">
         <v>67</v>
       </c>
+      <c r="E15" t="s">
+        <v>77</v>
+      </c>
     </row>
     <row r="16" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
       <c r="B16" t="s">
@@ -1440,8 +1465,11 @@
       <c r="D16" s="4" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>56</v>
       </c>
@@ -1451,8 +1479,11 @@
       <c r="D17" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>58</v>
       </c>
@@ -1461,12 +1492,26 @@
       </c>
       <c r="D18" t="s">
         <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19">
+        <v>660</v>
+      </c>
+      <c r="E19">
+        <v>672</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:K5 A19:B19 A12 C12 A13:C13 E13:K13 E12:K12 A14:C14 E14:K14 A15:B15 E15:K15 A16:B16 E16:K16 A17:B17 E17:K17 A18:B18 E18:K18 A20:B20 D20:K20 D19:K19 A9:B9 A7:B7 F7:K7 A8:B8 F8:K8 A11:B11 F11:K11 A10:B10 F10:K10 F9:K9 A6:B6 D6:K6" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:K5 A19 A12 C12 A13:C13 F13:K13 F12:K12 A14:C14 F14:K14 A15:B15 F15:K15 A16:B16 F16:K16 A17:B17 F17:K17 A18:B18 F18:K18 A20:B20 D20:K20 F19:K19 A9:B9 A7:B7 F7:K7 A8:B8 F8:K8 A11:B11 F11:K11 A10:B10 F10:K10 F9:K9 A6:B6 D6:K6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
se añade experimento 2
</commit_message>
<xml_diff>
--- a/Parametros_entrenamientos.xlsx
+++ b/Parametros_entrenamientos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28925"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\julio\Documents\VIU\2425\TFM\codigo\trabajo aprendizaje refuerzo\git\Proyecto_programacion_APR\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49149E8B-9DCE-4585-B535-E1C157E0D989}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96BE9284-518D-4A03-BFEC-9C52B3A20D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="78">
   <si>
     <t>PRUEBAS</t>
   </si>
@@ -214,9 +214,6 @@
   </si>
   <si>
     <t>500,000</t>
-  </si>
-  <si>
-    <t>0.97</t>
   </si>
   <si>
     <t>18 ~ 20 Mean 19,6_x000D_</t>
@@ -250,6 +247,18 @@
     <t xml:space="preserve">va subiendo un poco "linealmente"
 ligera mayor estabilidad que para los otros casos
 </t>
+  </si>
+  <si>
+    <t>num_episodes</t>
+  </si>
+  <si>
+    <t>112m 37 seg</t>
+  </si>
+  <si>
+    <t>7 ~ 23 | Media: 11.80</t>
+  </si>
+  <si>
+    <t>va subiendo mucho</t>
   </si>
 </sst>
 </file>
@@ -1030,7 +1039,7 @@
         <v>53</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G15" t="s">
         <v>53</v>
@@ -1059,7 +1068,7 @@
         <v>53</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G16" t="s">
         <v>53</v>
@@ -1142,10 +1151,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:K18"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:D18"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1154,7 +1163,8 @@
     <col min="2" max="2" width="22.3984375" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="42.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="30.796875" bestFit="1" customWidth="1"/>
-    <col min="5" max="11" width="14.296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.69921875" bestFit="1" customWidth="1"/>
+    <col min="6" max="11" width="14.296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.3">
@@ -1288,8 +1298,8 @@
       <c r="B6" t="s">
         <v>19</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
+      <c r="C6">
+        <v>4</v>
       </c>
       <c r="D6" t="s">
         <v>20</v>
@@ -1320,55 +1330,70 @@
       <c r="B7" t="s">
         <v>21</v>
       </c>
-      <c r="C7" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" t="s">
-        <v>22</v>
+      <c r="C7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="D7">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="E7" s="1">
+        <v>5.0000000000000002E-5</v>
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B8" t="s">
         <v>23</v>
       </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>64</v>
+      <c r="C8">
+        <v>0.99</v>
+      </c>
+      <c r="D8" s="1">
+        <v>0.97</v>
+      </c>
+      <c r="E8">
+        <v>0.99</v>
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="C9" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" t="s">
-        <v>26</v>
+      <c r="C9">
+        <v>10000</v>
+      </c>
+      <c r="D9">
+        <v>10000</v>
+      </c>
+      <c r="E9">
+        <v>10000</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" t="s">
-        <v>28</v>
+      <c r="C10">
+        <v>24</v>
+      </c>
+      <c r="D10">
+        <v>24</v>
+      </c>
+      <c r="E10">
+        <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:11" x14ac:dyDescent="0.3">
       <c r="B11" t="s">
         <v>29</v>
       </c>
-      <c r="C11" t="s">
-        <v>30</v>
-      </c>
-      <c r="D11" t="s">
-        <v>30</v>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="31.2" x14ac:dyDescent="0.3">
@@ -1376,13 +1401,16 @@
         <v>31</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C12" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>71</v>
+      </c>
+      <c r="E12" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:11" x14ac:dyDescent="0.3">
@@ -1390,10 +1418,13 @@
         <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D13" t="s">
-        <v>71</v>
+        <v>70</v>
+      </c>
+      <c r="E13" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="14" spans="1:11" x14ac:dyDescent="0.3">
@@ -1401,10 +1432,13 @@
         <v>50</v>
       </c>
       <c r="C14" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D14" t="s">
-        <v>67</v>
+        <v>66</v>
+      </c>
+      <c r="E14" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
@@ -1412,10 +1446,13 @@
         <v>52</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D15" s="4" t="s">
-        <v>68</v>
+        <v>67</v>
+      </c>
+      <c r="E15" t="s">
+        <v>77</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="46.8" x14ac:dyDescent="0.3">
@@ -1423,24 +1460,30 @@
         <v>55</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D16" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.3">
+        <v>67</v>
+      </c>
+      <c r="E16" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B17" t="s">
         <v>56</v>
       </c>
       <c r="C17" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.3">
+        <v>68</v>
+      </c>
+      <c r="E17" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
       <c r="B18" t="s">
         <v>58</v>
       </c>
@@ -1449,12 +1492,26 @@
       </c>
       <c r="D18" t="s">
         <v>59</v>
+      </c>
+      <c r="E18" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B19" t="s">
+        <v>74</v>
+      </c>
+      <c r="D19">
+        <v>660</v>
+      </c>
+      <c r="E19">
+        <v>672</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:K11 A19:B19 A12 C12 A13:C13 E13:K13 E12:K12 A14:C14 E14:K14 A15:B15 E15:K15 A16:B16 E16:K16 A17:B17 E17:K17 A18:B18 E18:K18 A20:B20 D20:K20 D19:K19" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:K5 A19 A12 C12 A13:C13 F13:K13 F12:K12 A14:C14 F14:K14 A15:B15 F15:K15 A16:B16 F16:K16 A17:B17 F17:K17 A18:B18 F18:K18 A20:B20 D20:K20 F19:K19 A9:B9 A7:B7 F7:K7 A8:B8 F8:K8 A11:B11 F11:K11 A10:B10 F10:K10 F9:K9 A6:B6 D6:K6" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>